<commit_message>
the actual 24 jun
</commit_message>
<xml_diff>
--- a/Daily_plan/2019/06_jun/June.xlsx
+++ b/Daily_plan/2019/06_jun/June.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Week_3" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Week_4" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="106">
   <si>
     <t xml:space="preserve">Week_03</t>
   </si>
@@ -167,6 +167,9 @@
     <t xml:space="preserve">An introduction to std::array</t>
   </si>
   <si>
+    <t xml:space="preserve">NYS</t>
+  </si>
+  <si>
     <t xml:space="preserve">An introduction to std::vector</t>
   </si>
   <si>
@@ -179,12 +182,18 @@
     <t xml:space="preserve">Stack using linked list using C</t>
   </si>
   <si>
+    <t xml:space="preserve">stack</t>
+  </si>
+  <si>
     <t xml:space="preserve">Stack using linked list using C++</t>
   </si>
   <si>
     <t xml:space="preserve">Queue using linked list using C</t>
   </si>
   <si>
+    <t xml:space="preserve">queue  </t>
+  </si>
+  <si>
     <t xml:space="preserve">Queue using linked list using C++</t>
   </si>
   <si>
@@ -254,9 +263,6 @@
     <t xml:space="preserve">20-06-2019</t>
   </si>
   <si>
-    <t xml:space="preserve">NYS</t>
-  </si>
-  <si>
     <t xml:space="preserve">Revised the project and technical part and went through the C++ topics</t>
   </si>
   <si>
@@ -299,31 +305,40 @@
     <t xml:space="preserve">Installing the python3.5, uninstall 2 and </t>
   </si>
   <si>
-    <t xml:space="preserve">Arrays (Part I)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arrays (Part II)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.7a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.8a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.8b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.9a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.11a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.12a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.x</t>
+    <t xml:space="preserve"> 24-06-2019 to 28-06-2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linked list to contain pointer to object instead of data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linked list using C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linked list using C++</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Circular linked list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binary Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24-06-2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Queue is performed using seperate iterator, Tried to overload -&gt; operator but didn’t succeed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int </t>
+  </si>
+  <si>
+    <t xml:space="preserve">scrum, python discussion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-06-2019</t>
   </si>
 </sst>
 </file>
@@ -334,7 +349,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0%"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -379,13 +394,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -482,7 +490,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -567,18 +575,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -658,19 +654,20 @@
   </sheetPr>
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.4642857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.4489795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.1122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.3673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1098,45 +1095,63 @@
       <c r="B23" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="11"/>
+      <c r="C23" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="E23" s="12" t="n">
         <v>0.5</v>
       </c>
-      <c r="F23" s="12"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F23" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="n">
         <v>21</v>
       </c>
       <c r="B24" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="11"/>
+      <c r="D24" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="E24" s="12" t="n">
         <v>0.5</v>
       </c>
-      <c r="F24" s="12"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F24" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="n">
         <v>22</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="11"/>
+        <v>50</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="E25" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="F25" s="12"/>
+      <c r="F25" s="12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4"/>
       <c r="B26" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
@@ -1148,10 +1163,14 @@
         <v>1</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="11"/>
+        <v>52</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="11" t="n">
+        <v>0.8</v>
+      </c>
       <c r="E27" s="12" t="n">
         <v>4</v>
       </c>
@@ -1159,54 +1178,70 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="n">
         <v>2</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="11"/>
+        <v>54</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="E28" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="F28" s="12"/>
+      <c r="F28" s="12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="n">
         <v>3</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="11"/>
+        <v>55</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="11" t="n">
+        <v>0.8</v>
+      </c>
       <c r="E29" s="12" t="n">
         <v>4</v>
       </c>
       <c r="F29" s="12" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="n">
         <v>4</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="11"/>
+        <v>57</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="E30" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="F30" s="12"/>
+      <c r="F30" s="12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4"/>
       <c r="B31" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="7"/>
@@ -1218,10 +1253,10 @@
         <v>1</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D32" s="11" t="n">
         <v>1</v>
@@ -1236,7 +1271,7 @@
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4"/>
       <c r="B33" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="7"/>
@@ -1248,19 +1283,23 @@
         <v>1</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C34" s="13"/>
-      <c r="D34" s="11"/>
+      <c r="D34" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="E34" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="F34" s="12"/>
+      <c r="F34" s="12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4"/>
       <c r="B35" s="14" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="7"/>
@@ -1272,15 +1311,17 @@
         <v>1</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C36" s="10"/>
-      <c r="D36" s="11"/>
+      <c r="D36" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="E36" s="12" t="n">
         <v>2.5</v>
       </c>
       <c r="F36" s="12" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1288,15 +1329,17 @@
         <v>2</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C37" s="10"/>
-      <c r="D37" s="11"/>
+      <c r="D37" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="E37" s="12" t="n">
         <v>4.5</v>
       </c>
       <c r="F37" s="12" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1306,15 +1349,15 @@
       </c>
       <c r="F38" s="0" t="n">
         <f aca="false">SUM(F3:F37)</f>
-        <v>26.6</v>
+        <v>32.1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1322,19 +1365,19 @@
         <v>2</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1354,45 +1397,63 @@
       <c r="B43" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C43" s="10"/>
-      <c r="D43" s="11"/>
+      <c r="C43" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="E43" s="12" t="n">
         <v>0.5</v>
       </c>
-      <c r="F43" s="12"/>
+      <c r="F43" s="12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="12" t="n">
         <v>2</v>
       </c>
       <c r="B44" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C44" s="10"/>
-      <c r="D44" s="11"/>
+      <c r="D44" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="E44" s="12" t="n">
         <v>0.5</v>
       </c>
-      <c r="F44" s="12"/>
+      <c r="F44" s="12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="12" t="n">
         <v>3</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C45" s="10"/>
-      <c r="D45" s="11"/>
+        <v>50</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="E45" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="F45" s="12"/>
+      <c r="F45" s="12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="12"/>
       <c r="B46" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C46" s="6"/>
       <c r="D46" s="7"/>
@@ -1404,47 +1465,63 @@
         <v>1</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C47" s="10"/>
-      <c r="D47" s="11"/>
+        <v>73</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="E47" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="F47" s="12"/>
+      <c r="F47" s="12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="12" t="n">
         <v>2</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C48" s="10"/>
-      <c r="D48" s="11"/>
+      <c r="D48" s="11" t="n">
+        <v>0.8</v>
+      </c>
       <c r="E48" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="F48" s="12"/>
+      <c r="F48" s="12" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="12" t="n">
         <v>3</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C49" s="10"/>
-      <c r="D49" s="11"/>
+        <v>75</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D49" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="E49" s="17" t="n">
         <v>1.5</v>
       </c>
-      <c r="F49" s="12"/>
+      <c r="F49" s="12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="12"/>
       <c r="B50" s="14" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C50" s="6"/>
       <c r="D50" s="7"/>
@@ -1456,10 +1533,10 @@
         <v>1</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D51" s="11" t="n">
         <v>1</v>
@@ -1476,12 +1553,14 @@
         <v>2</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D52" s="11"/>
+        <v>77</v>
+      </c>
+      <c r="D52" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="E52" s="12" t="n">
         <v>1</v>
       </c>
@@ -1498,7 +1577,7 @@
       </c>
       <c r="F53" s="20" t="n">
         <f aca="false">SUM(F42:F52)</f>
-        <v>3.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1509,10 +1588,10 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1520,19 +1599,19 @@
         <v>2</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1553,7 +1632,7 @@
         <v>47</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="D58" s="11" t="n">
         <v>0</v>
@@ -1570,10 +1649,10 @@
         <v>2</v>
       </c>
       <c r="B59" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C59" s="10" t="s">
         <v>48</v>
-      </c>
-      <c r="C59" s="10" t="s">
-        <v>77</v>
       </c>
       <c r="D59" s="11" t="n">
         <v>0</v>
@@ -1590,10 +1669,10 @@
         <v>3</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="D60" s="11" t="n">
         <v>0</v>
@@ -1608,7 +1687,7 @@
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="12"/>
       <c r="B61" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C61" s="6"/>
       <c r="D61" s="7"/>
@@ -1620,10 +1699,10 @@
         <v>1</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D62" s="11" t="n">
         <v>1</v>
@@ -1638,7 +1717,7 @@
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="12"/>
       <c r="B63" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C63" s="6"/>
       <c r="D63" s="7"/>
@@ -1650,10 +1729,10 @@
         <v>1</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="D64" s="11" t="n">
         <v>0</v>
@@ -1668,7 +1747,7 @@
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="12"/>
       <c r="B65" s="14" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C65" s="6"/>
       <c r="D65" s="7"/>
@@ -1680,10 +1759,10 @@
         <v>1</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D66" s="11" t="n">
         <v>1</v>
@@ -1700,10 +1779,10 @@
         <v>2</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C67" s="18" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D67" s="11" t="n">
         <v>1</v>
@@ -1735,10 +1814,10 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1746,19 +1825,19 @@
         <v>2</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E71" s="15" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F71" s="15" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1914,7 +1993,7 @@
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="12"/>
       <c r="B80" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C80" s="6"/>
       <c r="D80" s="7"/>
@@ -1926,10 +2005,10 @@
         <v>1</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C81" s="13" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D81" s="11" t="n">
         <v>0.7</v>
@@ -1944,7 +2023,7 @@
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="12"/>
       <c r="B82" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C82" s="6"/>
       <c r="D82" s="7"/>
@@ -1956,10 +2035,10 @@
         <v>1</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C83" s="13" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="D83" s="11" t="n">
         <v>0</v>
@@ -1974,7 +2053,7 @@
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="12"/>
       <c r="B84" s="14" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C84" s="6"/>
       <c r="D84" s="7"/>
@@ -1986,10 +2065,10 @@
         <v>1</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D85" s="11" t="n">
         <v>1</v>
@@ -2006,10 +2085,10 @@
         <v>2</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C86" s="18" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D86" s="11" t="n">
         <v>1</v>
@@ -2035,10 +2114,10 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2046,19 +2125,19 @@
         <v>2</v>
       </c>
       <c r="B90" s="15" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D90" s="15" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E90" s="15" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F90" s="15" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2194,7 +2273,7 @@
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="12"/>
       <c r="B98" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C98" s="6"/>
       <c r="D98" s="7"/>
@@ -2206,10 +2285,10 @@
         <v>1</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C99" s="13" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D99" s="11" t="n">
         <v>0.4</v>
@@ -2224,7 +2303,7 @@
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="12"/>
       <c r="B100" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C100" s="6"/>
       <c r="D100" s="7"/>
@@ -2236,10 +2315,10 @@
         <v>1</v>
       </c>
       <c r="B101" s="10" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C101" s="13" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="D101" s="11" t="n">
         <v>1</v>
@@ -2254,7 +2333,7 @@
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="12"/>
       <c r="B102" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C102" s="6"/>
       <c r="D102" s="7"/>
@@ -2266,10 +2345,10 @@
         <v>1</v>
       </c>
       <c r="B103" s="10" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C103" s="13" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="D103" s="11" t="n">
         <v>0</v>
@@ -2284,7 +2363,7 @@
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="12"/>
       <c r="B104" s="14" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C104" s="6"/>
       <c r="D104" s="7"/>
@@ -2296,10 +2375,10 @@
         <v>1</v>
       </c>
       <c r="B105" s="10" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C105" s="10" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D105" s="11" t="n">
         <v>1</v>
@@ -2316,10 +2395,10 @@
         <v>2</v>
       </c>
       <c r="B106" s="10" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C106" s="18" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D106" s="11" t="n">
         <v>1</v>
@@ -2345,10 +2424,10 @@
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2356,19 +2435,19 @@
         <v>2</v>
       </c>
       <c r="B110" s="15" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C110" s="15" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D110" s="15" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E110" s="15" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F110" s="15" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2504,7 +2583,7 @@
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="12"/>
       <c r="B118" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C118" s="6"/>
       <c r="D118" s="7"/>
@@ -2516,10 +2595,10 @@
         <v>1</v>
       </c>
       <c r="B119" s="10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C119" s="13" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="D119" s="11" t="n">
         <v>0</v>
@@ -2534,7 +2613,7 @@
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="12"/>
       <c r="B120" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C120" s="6"/>
       <c r="D120" s="7"/>
@@ -2546,10 +2625,10 @@
         <v>1</v>
       </c>
       <c r="B121" s="10" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C121" s="13" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D121" s="11"/>
       <c r="E121" s="17" t="n">
@@ -2562,7 +2641,7 @@
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="12"/>
       <c r="B122" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C122" s="6"/>
       <c r="D122" s="7"/>
@@ -2574,10 +2653,10 @@
         <v>1</v>
       </c>
       <c r="B123" s="10" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C123" s="13" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="D123" s="11" t="n">
         <v>0</v>
@@ -2592,7 +2671,7 @@
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="12"/>
       <c r="B124" s="14" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C124" s="6"/>
       <c r="D124" s="7"/>
@@ -2604,10 +2683,10 @@
         <v>1</v>
       </c>
       <c r="B125" s="10" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C125" s="10" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D125" s="11" t="n">
         <v>1</v>
@@ -2624,10 +2703,10 @@
         <v>2</v>
       </c>
       <c r="B126" s="10" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C126" s="18" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D126" s="11" t="n">
         <v>1</v>
@@ -2716,254 +2795,655 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.6377551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.43877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.1122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.3673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2551020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
-        <v>92</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="9" t="s">
-        <v>93</v>
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="21" t="n">
-        <v>6.3</v>
-      </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="9" t="s">
-        <v>11</v>
-      </c>
+      <c r="A3" s="4"/>
+      <c r="B3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="21" t="n">
-        <v>6.4</v>
-      </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="9" t="s">
-        <v>13</v>
-      </c>
+      <c r="A4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="21" t="n">
+      <c r="A5" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" s="12" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="F9" s="12"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4"/>
+      <c r="B15" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="12" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F16" s="12" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12" t="n">
+        <v>5</v>
+      </c>
+      <c r="F17" s="12" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="12" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F18" s="12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="0" t="n">
+        <f aca="false">SUM(E3:E17)</f>
+        <v>40</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <f aca="false">SUM(F3:F18)</f>
         <v>6.5</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="21" t="n">
-        <v>6.6</v>
-      </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="21" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="21" t="n">
-        <v>6.8</v>
-      </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="23" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="12"/>
+      <c r="B23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="16"/>
+    </row>
+    <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="11" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E24" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="F24" s="12" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="F25" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="12"/>
+      <c r="B26" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="16"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="12"/>
+      <c r="B28" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="16"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" s="12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F29" s="12" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" s="12" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" s="12" t="n">
+        <f aca="false">0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="F31" s="12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="E32" s="20" t="n">
+        <f aca="false">SUM(E23:E31)</f>
+        <v>8</v>
+      </c>
+      <c r="F32" s="20" t="n">
+        <f aca="false">SUM(F23:F31)</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="12"/>
+      <c r="B36" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="16"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="10"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F37" s="12"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="10"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="F38" s="12"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="B39" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="21" t="n">
-        <v>6.9</v>
-      </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="21" t="n">
-        <v>6.1</v>
-      </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="21" t="n">
-        <v>6.11</v>
-      </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="21" t="n">
-        <v>6.12</v>
-      </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="21" t="n">
-        <v>6.13</v>
-      </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="21" t="n">
-        <v>6.14</v>
-      </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="21" t="n">
-        <v>6.15</v>
-      </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="21" t="n">
-        <v>6.16</v>
-      </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="23" t="s">
+      <c r="C39" s="10"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F39" s="12"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="12"/>
+      <c r="B40" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="6"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="16"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="10"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F41" s="12"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="12"/>
+      <c r="B42" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" s="6"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="16"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="10"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F43" s="12"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="10"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F44" s="12"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="B45" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="9" t="s">
-        <v>49</v>
+      <c r="C45" s="18"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="12" t="n">
+        <f aca="false">0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="F45" s="12"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="E46" s="20" t="n">
+        <f aca="false">SUM(E36:E45)</f>
+        <v>8</v>
+      </c>
+      <c r="F46" s="20" t="n">
+        <f aca="false">SUM(F36:F45)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="Arrays (Part I)"/>
-    <hyperlink ref="C2" r:id="rId2" display="Arrays (Part II)"/>
-    <hyperlink ref="C3" r:id="rId3" display="Arrays and loops"/>
-    <hyperlink ref="C4" r:id="rId4" display="Sorting an array using selection sort"/>
-    <hyperlink ref="C5" r:id="rId5" display="Multidimensional arrays"/>
-    <hyperlink ref="C6" r:id="rId6" display="C-style strings"/>
-    <hyperlink ref="C7" r:id="rId7" display="Introduction to pointers"/>
-    <hyperlink ref="C8" r:id="rId8" display="Null pointers"/>
-    <hyperlink ref="C9" r:id="rId9" display="Pointers and arrays"/>
-    <hyperlink ref="C10" r:id="rId10" display="Pointer arithmetic and array indexing"/>
-    <hyperlink ref="C11" r:id="rId11" display="C-style string symbolic constants"/>
-    <hyperlink ref="C12" r:id="rId12" display="Dynamic memory allocation with new and delete"/>
-    <hyperlink ref="C13" r:id="rId13" display="Dynamically allocating arrays"/>
-    <hyperlink ref="C14" r:id="rId14" display="Pointers and const"/>
-    <hyperlink ref="C15" r:id="rId15" display="Reference variables"/>
-    <hyperlink ref="C16" r:id="rId16" display="References and const"/>
-    <hyperlink ref="C17" r:id="rId17" display="Member selection with pointers and references"/>
-    <hyperlink ref="C18" r:id="rId18" display="For each loops"/>
-    <hyperlink ref="C19" r:id="rId19" display="Void pointers"/>
-    <hyperlink ref="C20" r:id="rId20" display="Pointers to pointers and dynamic multidimensional arrays"/>
-    <hyperlink ref="C21" r:id="rId21" display="An introduction to std::array"/>
-    <hyperlink ref="C22" r:id="rId22" display="An introduction to std::vector"/>
-    <hyperlink ref="C23" r:id="rId23" display="Chapter 6 comprehensive quiz"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>